<commit_message>
Final coommited hybrid framwork.
</commit_message>
<xml_diff>
--- a/Selenium_demos/src/test/java/Excelfiles/test_data.xlsx
+++ b/Selenium_demos/src/test/java/Excelfiles/test_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>From City</t>
   </si>
@@ -36,12 +36,6 @@
     <t>LHR</t>
   </si>
   <si>
-    <t>12/15/2013</t>
-  </si>
-  <si>
-    <t>12/31/2013</t>
-  </si>
-  <si>
     <t>CDG</t>
   </si>
   <si>
@@ -49,6 +43,12 @@
   </si>
   <si>
     <t>MIL</t>
+  </si>
+  <si>
+    <t>12/15/2017</t>
+  </si>
+  <si>
+    <t>12/31/2017</t>
   </si>
 </sst>
 </file>
@@ -84,9 +84,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -408,73 +409,59 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>